<commit_message>
Bug Fixes Bonn - Part 2
- new code list for account assignment elements
- updated pipeline + dataset for 2016
</commit_message>
<xml_diff>
--- a/Bonn/raw/KostenartengruppeBonn2016.xlsx
+++ b/Bonn/raw/KostenartengruppeBonn2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ok-server\eis-homes\cengels\Desktop\GitHub\OpenBudgets\datasets\Bonn\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ok-server\EIS-Homes\cengels\Eigene Dateien\OpenBudgets.eu\DataSets\SampleData\Bonn\Raw Processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="546">
   <si>
     <t>Kostenart</t>
   </si>
@@ -1650,6 +1650,18 @@
   </si>
   <si>
     <t>ZeileInErgebnisplan</t>
+  </si>
+  <si>
+    <t>K11-281</t>
+  </si>
+  <si>
+    <t>Aufwendungen aus internen Leistungsbez.</t>
+  </si>
+  <si>
+    <t>K11-271</t>
+  </si>
+  <si>
+    <t>Erträge aus internen Leistungsbez.</t>
   </si>
 </sst>
 </file>
@@ -1659,7 +1671,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1670,6 +1682,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1717,7 +1736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1756,6 +1775,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2036,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G526"/>
+  <dimension ref="A1:H531"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A509" workbookViewId="0">
+      <selection activeCell="F520" sqref="F520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13935,7 +13957,48 @@
         <v>537</v>
       </c>
     </row>
+    <row r="527" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A527" s="7">
+        <v>27</v>
+      </c>
+      <c r="B527" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="C527" s="4"/>
+      <c r="D527" s="6"/>
+      <c r="E527" s="4"/>
+      <c r="F527" s="4" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A528" s="7">
+        <v>28</v>
+      </c>
+      <c r="B528" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="C528" s="4"/>
+      <c r="D528" s="6"/>
+      <c r="E528" s="4"/>
+      <c r="F528" s="4" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="530" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E530" s="19"/>
+      <c r="F530" s="20"/>
+      <c r="G530" s="18"/>
+    </row>
+    <row r="531" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F531" s="19"/>
+      <c r="G531" s="18"/>
+      <c r="H531" s="18"/>
+    </row>
   </sheetData>
+  <sortState ref="A527:H528">
+    <sortCondition ref="A527:A528"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>